<commit_message>
Se connecter à la BD et MDP Chiffré
</commit_message>
<xml_diff>
--- a/Ludotheque/gestion-projet/ProductBacklogV5.xlsx
+++ b/Ludotheque/gestion-projet/ProductBacklogV5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/inzo/Desktop/MesProjetsGIT/Ludotheque/gestion-projet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zelfakhadi2024\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCB97E20-4832-8A49-8356-5AAF92658693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843441A4-513D-4960-AD94-CC934F1AE00C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="17520" xr2:uid="{1FDB83B7-599D-4D42-AA13-F5EE32DADB90}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{1FDB83B7-599D-4D42-AA13-F5EE32DADB90}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
   <si>
     <t>PRODUCT BACKLOG LUDOTHEQUE</t>
   </si>
@@ -203,13 +203,37 @@
     <t>1.  Dépendance : spring-boot-starter-security : 
  par défaut et personnalisé
 2. implementation 'org.thymeleaf.extras:thymeleaf-extras-springsecurity6:3.1.2.RELEASE'  :</t>
+  </si>
+  <si>
+    <t>EN COURS</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">se connecter à partir des mots de passe de la BD Chiffré
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+MOT DE PASSE AZERTY encodé par le Prof
+A faire :
+- créer class de test 
+- afficher le mode de passe dans la console
+- encoder le mdt Azerty 
+- faire insert du mdp chiffré dans la BD</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,8 +270,14 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -257,12 +287,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -348,7 +372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -377,16 +401,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -408,21 +422,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -760,27 +767,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52D07A81-0E55-45DE-A090-3CCE23AAB227}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.5" style="6"/>
-    <col min="3" max="3" width="51.5" customWidth="1"/>
-    <col min="4" max="4" width="45.5" customWidth="1"/>
-    <col min="5" max="5" width="23.5" customWidth="1"/>
-    <col min="6" max="6" width="43.33203125" style="6" customWidth="1"/>
-    <col min="15" max="15" width="6.83203125" customWidth="1"/>
-    <col min="16" max="16" width="6.5" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" style="6"/>
+    <col min="3" max="3" width="51.42578125" customWidth="1"/>
+    <col min="4" max="4" width="45.42578125" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" customWidth="1"/>
+    <col min="6" max="6" width="43.42578125" style="6" customWidth="1"/>
+    <col min="15" max="15" width="6.85546875" customWidth="1"/>
+    <col min="16" max="16" width="6.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="34" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" ht="34.5" x14ac:dyDescent="0.55000000000000004">
       <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -794,11 +801,11 @@
         <v>4</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="21" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>3500</v>
       </c>
@@ -816,7 +823,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>3480</v>
       </c>
@@ -832,21 +839,21 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="25">
+    <row r="6" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
         <v>3470</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="28"/>
-      <c r="E6" s="25"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="2"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>3460</v>
       </c>
@@ -864,109 +871,111 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="25">
+    <row r="8" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>2899</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="28" t="s">
+      <c r="D8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="25"/>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="25">
+      <c r="E8" s="2"/>
+      <c r="F8" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>2889</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="25"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="2"/>
       <c r="F9" s="7"/>
     </row>
-    <row r="10" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="25">
+    <row r="10" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>2879</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="28"/>
-      <c r="E10" s="25"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="2"/>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="25">
+    <row r="11" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
         <v>2799</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="25"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="2"/>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="25">
+    <row r="12" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
         <v>2789</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="28"/>
-      <c r="E12" s="25"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="2"/>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="25">
+    <row r="13" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
         <v>2779</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="28"/>
-      <c r="E13" s="25"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="2"/>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="25">
+    <row r="14" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
         <v>2770</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="28"/>
-      <c r="E14" s="25" t="s">
+      <c r="D14" s="5"/>
+      <c r="E14" s="2" t="s">
         <v>30</v>
       </c>
       <c r="F14" s="7"/>
     </row>
-    <row r="15" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>2750</v>
       </c>
@@ -980,11 +989,11 @@
         <v>33</v>
       </c>
       <c r="E15" s="8"/>
-      <c r="F15" s="30" t="s">
+      <c r="F15" s="22" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="74" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>2740</v>
       </c>
@@ -998,21 +1007,23 @@
       <c r="E16" s="8"/>
       <c r="F16" s="9"/>
     </row>
-    <row r="17" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="12">
+    <row r="17" spans="1:6" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
         <v>2730</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="15"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="7"/>
-    </row>
-    <row r="18" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D17" s="11"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>1679</v>
       </c>
@@ -1026,7 +1037,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="7"/>
     </row>
-    <row r="19" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>1599</v>
       </c>
@@ -1040,7 +1051,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="7"/>
     </row>
-    <row r="20" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>1589</v>
       </c>
@@ -1054,7 +1065,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="7"/>
     </row>
-    <row r="21" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>960</v>
       </c>
@@ -1068,7 +1079,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="7"/>
     </row>
-    <row r="22" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>930</v>
       </c>
@@ -1082,7 +1093,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="7"/>
     </row>
-    <row r="23" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>920</v>
       </c>
@@ -1096,45 +1107,45 @@
       <c r="E23" s="2"/>
       <c r="F23" s="7"/>
     </row>
-    <row r="24" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="19">
+    <row r="24" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="15">
         <v>910</v>
       </c>
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C24" s="21" t="s">
+      <c r="C24" s="17" t="s">
         <v>51</v>
       </c>
       <c r="D24" s="5"/>
       <c r="E24" s="2"/>
       <c r="F24" s="7"/>
     </row>
-    <row r="25" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="16"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="18"/>
+    <row r="25" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="12"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="12"/>
+      <c r="D25" s="14"/>
       <c r="E25" s="2"/>
       <c r="F25" s="7"/>
     </row>
-    <row r="26" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="16"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="18"/>
+    <row r="26" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="12"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="14"/>
       <c r="E26" s="2"/>
       <c r="F26" s="7"/>
     </row>
-    <row r="27" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="22"/>
-      <c r="B27" s="23"/>
-      <c r="C27" s="24"/>
+    <row r="27" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="18"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="20"/>
       <c r="D27" s="5"/>
       <c r="E27" s="2"/>
       <c r="F27" s="7"/>
     </row>
-    <row r="28" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="7"/>
       <c r="C28" s="3"/>
@@ -1142,7 +1153,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="7"/>
     </row>
-    <row r="29" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="7"/>
       <c r="C29" s="3"/>
@@ -1150,7 +1161,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="7"/>
     </row>
-    <row r="30" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="7"/>
       <c r="C30" s="3"/>
@@ -1158,7 +1169,7 @@
       <c r="E30" s="2"/>
       <c r="F30" s="7"/>
     </row>
-    <row r="31" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="7"/>
       <c r="C31" s="3"/>
@@ -1166,7 +1177,7 @@
       <c r="E31" s="2"/>
       <c r="F31" s="7"/>
     </row>
-    <row r="32" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="7"/>
       <c r="C32" s="3"/>
@@ -1174,7 +1185,7 @@
       <c r="E32" s="2"/>
       <c r="F32" s="7"/>
     </row>
-    <row r="33" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="7"/>
       <c r="C33" s="3"/>
@@ -1182,7 +1193,7 @@
       <c r="E33" s="2"/>
       <c r="F33" s="7"/>
     </row>
-    <row r="34" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="7"/>
       <c r="C34" s="3"/>
@@ -1190,7 +1201,7 @@
       <c r="E34" s="2"/>
       <c r="F34" s="7"/>
     </row>
-    <row r="35" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="7"/>
       <c r="C35" s="3"/>

</xml_diff>